<commit_message>
update manual data compiled by resi
</commit_message>
<xml_diff>
--- a/data-raw/2020_09_17 MIP_SGP_variables.xlsx
+++ b/data-raw/2020_09_17 MIP_SGP_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graebnerc/icae-server/ICAE-Projekte-laufend/SPACE/Arbeitspakete/WP2/Variablen/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/develop/packages/competitivenessData/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388BF76C-65BF-054E-A259-A8C9C03C4B01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DAC9CB4-C01C-2F48-B29F-CD6D39EDBB31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="18240" tabRatio="891" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19980" yWindow="17120" windowWidth="20740" windowHeight="11760" tabRatio="891" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MIS-Indicator" sheetId="1" r:id="rId1"/>
@@ -18,15 +18,15 @@
     <sheet name="SGP-Compliance-Indicator" sheetId="6" r:id="rId3"/>
     <sheet name="Notes-to-MIS-Indicator" sheetId="4" r:id="rId4"/>
     <sheet name="Notes-to-SGP-EDP-Indicator" sheetId="5" r:id="rId5"/>
-    <sheet name="Abbreviations of Countries" sheetId="2" r:id="rId6"/>
-    <sheet name="Notes-to-SGP-Compliance-Indicat" sheetId="7" r:id="rId7"/>
+    <sheet name="Notes-to-SGP-Compliance-Indicat" sheetId="7" r:id="rId6"/>
+    <sheet name="Abbreviations of Countries" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="89">
   <si>
     <t>Member States</t>
   </si>
@@ -211,9 +211,6 @@
     <t>no IDR</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>IDR with excessive imbalances</t>
   </si>
   <si>
@@ -244,66 +241,6 @@
     <t>Country</t>
   </si>
   <si>
-    <t>MIP_2012</t>
-  </si>
-  <si>
-    <t>MIP_2013</t>
-  </si>
-  <si>
-    <t>MIP_2014</t>
-  </si>
-  <si>
-    <t>MIP_2015</t>
-  </si>
-  <si>
-    <t>MIP_2016</t>
-  </si>
-  <si>
-    <t>MIP_2017</t>
-  </si>
-  <si>
-    <t>MIP_2018</t>
-  </si>
-  <si>
-    <t>MIP_2019</t>
-  </si>
-  <si>
-    <t>MIP_2020</t>
-  </si>
-  <si>
-    <t>EDP_2009</t>
-  </si>
-  <si>
-    <t>EDP_2010</t>
-  </si>
-  <si>
-    <t>EDP_2011</t>
-  </si>
-  <si>
-    <t>EDP_2012</t>
-  </si>
-  <si>
-    <t>EDP_2013</t>
-  </si>
-  <si>
-    <t>EDP_2014</t>
-  </si>
-  <si>
-    <t>EDP_2015</t>
-  </si>
-  <si>
-    <t>EDP_2016</t>
-  </si>
-  <si>
-    <t>EDP_2017</t>
-  </si>
-  <si>
-    <t>EDP_2018</t>
-  </si>
-  <si>
-    <t>EDP_2019</t>
-  </si>
-  <si>
     <t>n</t>
   </si>
   <si>
@@ -319,9 +256,6 @@
     <t>UK has EDP from 2008-2014</t>
   </si>
   <si>
-    <t>kA</t>
-  </si>
-  <si>
     <t xml:space="preserve">categories: </t>
   </si>
   <si>
@@ -337,27 +271,9 @@
     <t>risk of non-compliance</t>
   </si>
   <si>
-    <t>SGP-Compliance_2015</t>
-  </si>
-  <si>
-    <t>SGP-Compliance_2016</t>
-  </si>
-  <si>
-    <t>SGP-Compliance_2017</t>
-  </si>
-  <si>
-    <t>SGP-Compliance_2018</t>
-  </si>
-  <si>
-    <t>SGP-Compliance_2019</t>
-  </si>
-  <si>
     <t>no DBP submitted yet</t>
   </si>
   <si>
-    <t>SGP-Compliance_2014</t>
-  </si>
-  <si>
     <t>titel of the column in Public Finances in EMU:</t>
   </si>
   <si>
@@ -373,10 +289,10 @@
     <t>particularly serious non-compliance</t>
   </si>
   <si>
-    <t>risk of non-compliance of non-compliance</t>
-  </si>
-  <si>
-    <t>broadly compliant compliant</t>
+    <t>NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">risk of non-compliance </t>
   </si>
 </sst>
 </file>
@@ -818,57 +734,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:J37"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A30"/>
+    <sheetView topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.33203125" customWidth="1"/>
-    <col min="5" max="5" width="35.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" customWidth="1"/>
-    <col min="9" max="9" width="23.1640625" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="5.83203125" customWidth="1"/>
+    <col min="3" max="3" width="5.5" customWidth="1"/>
+    <col min="4" max="4" width="8.5" customWidth="1"/>
+    <col min="5" max="5" width="5.1640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" customWidth="1"/>
+    <col min="7" max="7" width="8.5" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
+    <col min="10" max="10" width="49.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>80</v>
+    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="3">
+        <v>2012</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2013</v>
+      </c>
+      <c r="D1" s="3">
+        <v>2014</v>
+      </c>
+      <c r="E1" s="4">
+        <v>2015</v>
+      </c>
+      <c r="F1" s="3">
+        <v>2016</v>
+      </c>
+      <c r="G1" s="3">
+        <v>2017</v>
+      </c>
+      <c r="H1" s="3">
+        <v>2018</v>
+      </c>
+      <c r="I1" s="3">
+        <v>2019</v>
+      </c>
+      <c r="J1" s="3">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>59</v>
@@ -880,68 +832,68 @@
         <v>59</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" t="s">
         <v>63</v>
-      </c>
-      <c r="G3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I3" t="s">
-        <v>60</v>
-      </c>
-      <c r="J3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>60</v>
@@ -964,39 +916,39 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" t="s">
+        <v>59</v>
+      </c>
+      <c r="J6" t="s">
         <v>63</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" t="s">
-        <v>60</v>
-      </c>
-      <c r="G6" t="s">
-        <v>60</v>
-      </c>
-      <c r="H6" t="s">
-        <v>60</v>
-      </c>
-      <c r="I6" t="s">
-        <v>60</v>
-      </c>
-      <c r="J6" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
         <v>60</v>
@@ -1005,62 +957,62 @@
         <v>60</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F7" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" t="s">
+        <v>59</v>
+      </c>
+      <c r="J8" t="s">
         <v>63</v>
-      </c>
-      <c r="G8" t="s">
-        <v>60</v>
-      </c>
-      <c r="H8" t="s">
-        <v>60</v>
-      </c>
-      <c r="I8" t="s">
-        <v>60</v>
-      </c>
-      <c r="J8" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
         <v>58</v>
@@ -1068,81 +1020,81 @@
       <c r="C9" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>67</v>
+      <c r="D9" t="s">
+        <v>58</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="F9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I9" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="J9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" t="s">
-        <v>58</v>
+        <v>61</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="F10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
         <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H11" t="s">
         <v>59</v>
@@ -1151,140 +1103,140 @@
         <v>59</v>
       </c>
       <c r="J11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>67</v>
+        <v>87</v>
+      </c>
+      <c r="D12" t="s">
+        <v>61</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H12" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I12" t="s">
         <v>59</v>
       </c>
       <c r="J12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" t="s">
         <v>61</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D13" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="F13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I13" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="J13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
         <v>59</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J15" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
         <v>60</v>
@@ -1316,7 +1268,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
         <v>60</v>
@@ -1325,7 +1277,7 @@
         <v>60</v>
       </c>
       <c r="D17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>60</v>
@@ -1348,22 +1300,22 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G18" t="s">
         <v>60</v>
@@ -1380,22 +1332,22 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C19" t="s">
         <v>59</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F19" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G19" t="s">
         <v>60</v>
@@ -1412,7 +1364,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
         <v>60</v>
@@ -1421,62 +1373,62 @@
         <v>59</v>
       </c>
       <c r="D20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" t="s">
+        <v>59</v>
+      </c>
+      <c r="H20" t="s">
+        <v>59</v>
+      </c>
+      <c r="I20" t="s">
+        <v>59</v>
+      </c>
+      <c r="J20" t="s">
         <v>63</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F20" t="s">
-        <v>60</v>
-      </c>
-      <c r="G20" t="s">
-        <v>60</v>
-      </c>
-      <c r="H20" t="s">
-        <v>60</v>
-      </c>
-      <c r="I20" t="s">
-        <v>60</v>
-      </c>
-      <c r="J20" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
         <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G21" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H21" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I21" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J21" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B22" t="s">
         <v>60</v>
@@ -1491,7 +1443,7 @@
         <v>60</v>
       </c>
       <c r="F22" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G22" t="s">
         <v>60</v>
@@ -1508,39 +1460,39 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F23" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G23" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J23" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
         <v>58</v>
@@ -1552,80 +1504,80 @@
         <v>58</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F24" t="s">
         <v>62</v>
       </c>
       <c r="G24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H24" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I24" t="s">
         <v>59</v>
       </c>
       <c r="J24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D25" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="F25" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H25" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I25" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J25" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="F26" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G26" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I26" t="s">
         <v>60</v>
@@ -1636,25 +1588,25 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G27" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H27" t="s">
         <v>60</v>
@@ -1668,7 +1620,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B28" t="s">
         <v>59</v>
@@ -1686,21 +1638,21 @@
         <v>59</v>
       </c>
       <c r="G28" t="s">
+        <v>59</v>
+      </c>
+      <c r="H28" t="s">
+        <v>59</v>
+      </c>
+      <c r="I28" t="s">
+        <v>59</v>
+      </c>
+      <c r="J28" t="s">
         <v>63</v>
-      </c>
-      <c r="H28" t="s">
-        <v>60</v>
-      </c>
-      <c r="I28" t="s">
-        <v>60</v>
-      </c>
-      <c r="J28" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
         <v>59</v>
@@ -1715,58 +1667,26 @@
         <v>59</v>
       </c>
       <c r="F29" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J29" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>57</v>
-      </c>
-      <c r="B30" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" t="s">
-        <v>59</v>
-      </c>
-      <c r="D30" t="s">
-        <v>59</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G30" t="s">
-        <v>60</v>
-      </c>
-      <c r="H30" t="s">
-        <v>60</v>
-      </c>
-      <c r="I30" t="s">
-        <v>60</v>
-      </c>
-      <c r="J30" t="s">
-        <v>60</v>
-      </c>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1778,48 +1698,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I1" t="s">
-        <v>88</v>
-      </c>
-      <c r="J1" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" t="s">
-        <v>90</v>
-      </c>
-      <c r="L1" t="s">
-        <v>91</v>
+        <v>70</v>
+      </c>
+      <c r="B1">
+        <v>2009</v>
+      </c>
+      <c r="C1">
+        <v>2010</v>
+      </c>
+      <c r="D1">
+        <v>2011</v>
+      </c>
+      <c r="E1">
+        <v>2012</v>
+      </c>
+      <c r="F1">
+        <v>2013</v>
+      </c>
+      <c r="G1">
+        <v>2014</v>
+      </c>
+      <c r="H1">
+        <v>2015</v>
+      </c>
+      <c r="I1">
+        <v>2016</v>
+      </c>
+      <c r="J1">
+        <v>2017</v>
+      </c>
+      <c r="K1">
+        <v>2018</v>
+      </c>
+      <c r="L1">
+        <v>2019</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -1827,37 +1747,37 @@
         <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F2" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="H2" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="I2" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="J2" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="K2" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="L2" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -1865,37 +1785,37 @@
         <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D3" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E3" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F3" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="G3" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="H3" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="I3" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="J3" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="K3" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="L3" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -1903,37 +1823,37 @@
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D4" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F4" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="G4" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="H4" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="I4" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="J4" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="K4" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="L4" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -1941,37 +1861,37 @@
         <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E5" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F5" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="G5" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="H5" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="I5" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="J5" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="K5" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="L5" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1979,37 +1899,37 @@
         <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D6" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F6" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="G6" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="H6" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="I6" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="J6" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="K6" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="L6" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -2017,37 +1937,37 @@
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D7" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E7" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="F7" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G7" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="H7" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="I7" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="J7" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="K7" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="L7" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -2055,37 +1975,37 @@
         <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="C8" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D8" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E8" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F8" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="G8" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="H8" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="I8" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="J8" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="K8" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="L8" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -2093,37 +2013,37 @@
         <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="C9" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D9" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E9" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F9" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="G9" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="H9" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="I9" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="J9" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="K9" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="L9" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -2131,37 +2051,37 @@
         <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D10" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E10" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F10" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="G10" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="H10" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="I10" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="J10" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="K10" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="L10" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -2169,37 +2089,37 @@
         <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="C11" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D11" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E11" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F11" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="G11" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="H11" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="I11" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="J11" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="K11" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="L11" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -2207,37 +2127,37 @@
         <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="E12" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="F12" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="G12" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="H12" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="I12" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="J12" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="K12" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="L12" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -2245,37 +2165,37 @@
         <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="C13" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D13" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E13" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F13" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="G13" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="H13" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="I13" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="J13" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="K13" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="L13" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -2283,37 +2203,37 @@
         <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D14" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E14" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F14" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="G14" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="H14" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="I14" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="J14" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="K14" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="L14" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -2321,37 +2241,37 @@
         <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D15" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E15" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F15" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="G15" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="H15" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="I15" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="J15" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="K15" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="L15" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -2359,37 +2279,37 @@
         <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="C16" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D16" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E16" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F16" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="G16" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="H16" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="I16" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="J16" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="K16" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="L16" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -2397,37 +2317,37 @@
         <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C17" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D17" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E17" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="F17" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G17" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="H17" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="I17" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="J17" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="K17" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="L17" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -2435,37 +2355,37 @@
         <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="C18" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D18" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E18" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F18" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="G18" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="H18" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="I18" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="J18" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="K18" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="L18" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -2473,37 +2393,37 @@
         <v>47</v>
       </c>
       <c r="B19" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="C19" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D19" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E19" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F19" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="G19" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="H19" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="I19" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="J19" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="K19" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="L19" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -2511,37 +2431,37 @@
         <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D20" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E20" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F20" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="G20" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="H20" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="I20" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="J20" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="K20" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="L20" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -2549,37 +2469,37 @@
         <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="C21" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D21" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E21" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F21" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="G21" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="H21" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="I21" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="J21" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="K21" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="L21" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -2587,37 +2507,37 @@
         <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="C22" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D22" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E22" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F22" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="G22" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="H22" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="I22" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="J22" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="K22" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="L22" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -2625,37 +2545,37 @@
         <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D23" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E23" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F23" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="G23" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="H23" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="I23" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="J23" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="K23" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="L23" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -2663,37 +2583,37 @@
         <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="C24" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D24" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E24" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F24" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="G24" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="H24" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="I24" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="J24" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="K24" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="L24" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
@@ -2701,37 +2621,37 @@
         <v>53</v>
       </c>
       <c r="B25" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="C25" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D25" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E25" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F25" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="G25" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="H25" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="I25" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="J25" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="K25" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="L25" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
@@ -2739,37 +2659,37 @@
         <v>54</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="C26" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D26" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E26" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F26" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="G26" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="H26" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="I26" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="J26" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="K26" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="L26" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
@@ -2777,37 +2697,37 @@
         <v>55</v>
       </c>
       <c r="B27" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="C27" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D27" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E27" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="F27" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="G27" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="H27" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="I27" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="J27" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="K27" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="L27" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
@@ -2815,37 +2735,37 @@
         <v>56</v>
       </c>
       <c r="B28" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C28" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D28" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E28" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="F28" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G28" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="H28" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="I28" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="J28" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="K28" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="L28" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -2853,37 +2773,37 @@
         <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="C29" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D29" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E29" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F29" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="G29" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="H29" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="I29" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="J29" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="K29" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="L29" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2895,33 +2815,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" customWidth="1"/>
+    <col min="6" max="6" width="22.5" customWidth="1"/>
+    <col min="7" max="7" width="42.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>107</v>
+        <v>70</v>
+      </c>
+      <c r="B2">
+        <v>2014</v>
+      </c>
+      <c r="C2">
+        <v>2015</v>
+      </c>
+      <c r="D2">
+        <v>2016</v>
+      </c>
+      <c r="E2">
+        <v>2017</v>
+      </c>
+      <c r="F2">
+        <v>2018</v>
+      </c>
+      <c r="G2">
+        <v>2019</v>
       </c>
       <c r="H2" s="3"/>
     </row>
@@ -2930,22 +2858,22 @@
         <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="C3" t="s">
-        <v>116</v>
+        <v>79</v>
       </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="E3" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="F3" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="G3" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -2953,22 +2881,22 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E4" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="F4" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G4" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -2976,22 +2904,22 @@
         <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E5" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="F5" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G5" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -2999,22 +2927,22 @@
         <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="F6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -3022,22 +2950,22 @@
         <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="D7" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="E7" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="F7" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="G7" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -3045,22 +2973,22 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="C8" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="E8" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="F8" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="G8" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -3068,22 +2996,22 @@
         <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>116</v>
+        <v>79</v>
       </c>
       <c r="D9" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="E9" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="F9" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="G9" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -3091,16 +3019,22 @@
         <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
-        <v>97</v>
+        <v>87</v>
+      </c>
+      <c r="D10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" t="s">
+        <v>87</v>
       </c>
       <c r="F10" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="G10" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -3108,22 +3042,22 @@
         <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="E11" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="F11" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="G11" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -3131,22 +3065,22 @@
         <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="C12" t="s">
-        <v>116</v>
+        <v>79</v>
       </c>
       <c r="D12" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="E12" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="F12" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="G12" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -3154,22 +3088,22 @@
         <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C13" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D13" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E13" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="F13" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G13" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -3177,22 +3111,22 @@
         <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="C14" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="D14" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="E14" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="F14" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="G14" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -3200,22 +3134,22 @@
         <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C15" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D15" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="E15" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="F15" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="G15" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -3223,22 +3157,22 @@
         <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="C16" t="s">
-        <v>116</v>
+        <v>79</v>
       </c>
       <c r="D16" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="E16" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="F16" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="G16" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -3246,22 +3180,22 @@
         <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C17" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="D17" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="E17" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="F17" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="G17" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -3269,22 +3203,22 @@
         <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="C18" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="D18" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="E18" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="F18" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="G18" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -3292,22 +3226,22 @@
         <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D19" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E19" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="F19" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G19" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -3315,22 +3249,22 @@
         <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="C20" t="s">
-        <v>116</v>
+        <v>79</v>
       </c>
       <c r="D20" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="E20" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="F20" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="G20" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -3338,22 +3272,22 @@
         <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="D21" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="E21" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="F21" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="G21" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -3361,22 +3295,22 @@
         <v>49</v>
       </c>
       <c r="B22" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="C22" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="D22" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="E22" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="F22" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="G22" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -3384,22 +3318,22 @@
         <v>50</v>
       </c>
       <c r="B23" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C23" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D23" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E23" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="F23" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G23" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -3407,22 +3341,22 @@
         <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="D24" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="E24" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="F24" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="G24" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -3430,22 +3364,22 @@
         <v>52</v>
       </c>
       <c r="B25" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C25" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D25" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E25" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="F25" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G25" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -3453,22 +3387,22 @@
         <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="C26" t="s">
-        <v>116</v>
+        <v>79</v>
       </c>
       <c r="D26" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="E26" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="F26" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="G26" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -3476,22 +3410,22 @@
         <v>54</v>
       </c>
       <c r="B27" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="C27" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="D27" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="E27" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="F27" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="G27" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -3499,22 +3433,22 @@
         <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="C28" t="s">
-        <v>116</v>
+        <v>79</v>
       </c>
       <c r="D28" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="E28" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="F28" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="G28" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -3522,22 +3456,22 @@
         <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C29" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D29" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E29" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="F29" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G29" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -3545,22 +3479,22 @@
         <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C30" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D30" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E30" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="F30" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G30" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -3580,7 +3514,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -3606,7 +3540,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -3632,7 +3566,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -3646,7 +3580,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -3675,32 +3609,32 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3710,6 +3644,44 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:A31"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -3765,7 +3737,7 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
@@ -3871,44 +3843,6 @@
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rebuild data from scratch to make update effective
</commit_message>
<xml_diff>
--- a/data-raw/2020_09_17 MIP_SGP_variables.xlsx
+++ b/data-raw/2020_09_17 MIP_SGP_variables.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/develop/packages/competitivenessData/data-raw/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DAC9CB4-C01C-2F48-B29F-CD6D39EDBB31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19980" yWindow="17120" windowWidth="20740" windowHeight="11760" tabRatio="891" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="20730" windowHeight="11760" tabRatio="891" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="MIS-Indicator" sheetId="1" r:id="rId1"/>
@@ -298,7 +292,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -398,7 +392,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -414,9 +408,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -454,9 +448,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -489,26 +483,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -541,26 +518,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -733,25 +693,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="2" max="2" width="5.83203125" customWidth="1"/>
-    <col min="3" max="3" width="5.5" customWidth="1"/>
-    <col min="4" max="4" width="8.5" customWidth="1"/>
-    <col min="5" max="5" width="5.1640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="7.1640625" customWidth="1"/>
-    <col min="7" max="7" width="8.5" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" customWidth="1"/>
-    <col min="10" max="10" width="49.83203125" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="10" max="10" width="49.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1330,7 +1290,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -1362,7 +1322,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -1394,7 +1354,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1426,7 +1386,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -1458,7 +1418,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -1490,7 +1450,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -1522,7 +1482,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -1554,7 +1514,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -1586,7 +1546,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -1618,7 +1578,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -1650,7 +1610,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -1682,10 +1642,10 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
     </row>
   </sheetData>
@@ -1695,14 +1655,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -2578,7 +2538,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -2616,7 +2576,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -2654,7 +2614,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -2692,7 +2652,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -2730,7 +2690,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -2768,7 +2728,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -2812,21 +2772,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="29.83203125" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" customWidth="1"/>
-    <col min="6" max="6" width="22.5" customWidth="1"/>
-    <col min="7" max="7" width="42.5" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
+    <col min="7" max="7" width="42.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -3336,7 +3296,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -3359,7 +3319,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>52</v>
       </c>
@@ -3382,7 +3342,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -3405,7 +3365,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -3428,7 +3388,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>55</v>
       </c>
@@ -3451,7 +3411,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -3474,7 +3434,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -3503,14 +3463,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
@@ -3598,14 +3558,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -3643,14 +3603,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -3681,14 +3641,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A31"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>